<commit_message>
Add Devis function and code cleaning for the main window waiting for a rework.
</commit_message>
<xml_diff>
--- a/Agenda/modele_facture.xlsx
+++ b/Agenda/modele_facture.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Agenda\Agenda\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -119,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
@@ -360,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -378,36 +383,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,43 +391,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -472,12 +417,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -492,6 +431,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -501,14 +443,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,6 +518,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -567,7 +569,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,9 +602,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,6 +654,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -813,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,60 +864,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>63400</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -897,310 +933,378 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="30"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="45"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="19">
-        <v>300000</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="18"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="1"/>
       <c r="I11" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="42"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="22">
+        <f>F14*G14</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="43"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="22">
+        <f t="shared" ref="H15:H28" si="0">F15*G15</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="43"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="43"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="43"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="43"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="43"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="43"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="43"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="43"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="43"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="43"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="43"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="43"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="51"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="44"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="F29" s="49" t="s">
+      <c r="B29" s="51"/>
+      <c r="C29" s="52"/>
+      <c r="F29" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G29" s="50"/>
-      <c r="H29" s="48"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="26">
+        <f>SUM(H14:H28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="F30" s="49" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="F30" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="50"/>
-      <c r="H30" s="48"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="49" t="s">
+      <c r="F31" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="50"/>
-      <c r="H31" s="48"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F32" s="49" t="s">
+      <c r="F32" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="50"/>
-      <c r="H32" s="48"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="26"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F33" s="49" t="s">
+      <c r="F33" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="50"/>
-      <c r="H33" s="48"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="26"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F34" s="49" t="s">
+      <c r="F34" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="50"/>
-      <c r="H34" s="48"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F35" s="49" t="s">
+      <c r="F35" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G35" s="50"/>
-      <c r="H35" s="48"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="26">
+        <f>SUM(H29:H34)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="11">
         <v>0.2</v>
       </c>
-      <c r="H36" s="48"/>
+      <c r="H36" s="26">
+        <f>H35*G36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F37" s="49" t="s">
+      <c r="F37" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="50"/>
-      <c r="H37" s="48"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="26">
+        <f>H35+H36</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:H4"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A30:C30"/>
@@ -1217,19 +1321,6 @@
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E2:H4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.13541666666666666" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>